<commit_message>
add nwocasts for 2025q4
</commit_message>
<xml_diff>
--- a/Nowcasts/2025Q4/tables/nowcasts_2025Q4_Nr10_Np1_Nj0.xlsx
+++ b/Nowcasts/2025Q4/tables/nowcasts_2025Q4_Nr10_Np1_Nj0.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Row</t>
   </si>
@@ -109,6 +109,57 @@
   </si>
   <si>
     <t>2025-11-15</t>
+  </si>
+  <si>
+    <t>Prognose</t>
+  </si>
+  <si>
+    <t>surveys</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>turnover</t>
+  </si>
+  <si>
+    <t>financial</t>
+  </si>
+  <si>
+    <t>labor market</t>
+  </si>
+  <si>
+    <t>prices</t>
+  </si>
+  <si>
+    <t>national accounts</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>2025-09-30</t>
+  </si>
+  <si>
+    <t>2025-10-15</t>
+  </si>
+  <si>
+    <t>2025-10-30</t>
+  </si>
+  <si>
+    <t>2025-11-15</t>
+  </si>
+  <si>
+    <t>2025-11-30</t>
+  </si>
+  <si>
+    <t>2025-12-15</t>
   </si>
   <si>
     <t>Prognose</t>
@@ -189,58 +240,58 @@
   <cols>
     <col min="1" max="1" width="10.37890625" customWidth="true"/>
     <col min="2" max="2" width="12.64453125" customWidth="true"/>
-    <col min="3" max="3" width="14.24609375" customWidth="true"/>
-    <col min="4" max="4" width="14.24609375" customWidth="true"/>
-    <col min="5" max="5" width="16.24609375" customWidth="true"/>
-    <col min="6" max="6" width="15.64453125" customWidth="true"/>
+    <col min="3" max="3" width="13.64453125" customWidth="true"/>
+    <col min="4" max="4" width="13.64453125" customWidth="true"/>
+    <col min="5" max="5" width="14.64453125" customWidth="true"/>
+    <col min="6" max="6" width="15.24609375" customWidth="true"/>
     <col min="7" max="7" width="14.64453125" customWidth="true"/>
-    <col min="8" max="8" width="16.24609375" customWidth="true"/>
+    <col min="8" max="8" width="15.64453125" customWidth="true"/>
     <col min="9" max="9" width="15.24609375" customWidth="true"/>
-    <col min="10" max="10" width="15.1796875" customWidth="true"/>
-    <col min="11" max="11" width="15.77734375" customWidth="true"/>
+    <col min="10" max="10" width="15.046875" customWidth="true"/>
+    <col min="11" max="11" width="16.24609375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B2" s="0">
-        <v>0.21013678854266826</v>
+        <v>0.23088412219454385</v>
       </c>
       <c r="C2" s="0">
         <v>0</v>
@@ -272,177 +323,177 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B3" s="0">
-        <v>0.23717142787617834</v>
+        <v>0.30355597489376918</v>
       </c>
       <c r="C3" s="0">
         <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>0.013573763961064706</v>
+        <v>0.033256522344220912</v>
       </c>
       <c r="E3" s="0">
-        <v>-0.005866550256624456</v>
+        <v>0.0026443051604739211</v>
       </c>
       <c r="F3" s="0">
-        <v>0.0059959595854465675</v>
+        <v>0.036480476652970661</v>
       </c>
       <c r="G3" s="0">
-        <v>0.0087064951743055299</v>
+        <v>0.0055220178538752983</v>
       </c>
       <c r="H3" s="0">
-        <v>-0.00017291961727999134</v>
+        <v>0.0009315466554420393</v>
       </c>
       <c r="I3" s="0">
-        <v>0.0047363594655821179</v>
+        <v>-0.0056395971915511756</v>
       </c>
       <c r="J3" s="0">
         <v>0</v>
       </c>
       <c r="K3" s="0">
-        <v>6.1531021015609477e-05</v>
+        <v>-0.00052341877620631916</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0">
-        <v>0.32240686991988826</v>
+        <v>0.58608758295451224</v>
       </c>
       <c r="C4" s="0">
-        <v>0.066689185791222891</v>
+        <v>0.12646073831289756</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
       </c>
       <c r="E4" s="0">
-        <v>-0.00030477677907491231</v>
+        <v>0.0050078994482244702</v>
       </c>
       <c r="F4" s="0">
-        <v>0.00095722923606939144</v>
+        <v>-0.0011012920423843376</v>
       </c>
       <c r="G4" s="0">
         <v>0</v>
       </c>
       <c r="H4" s="0">
-        <v>-0.00016770444057367259</v>
+        <v>-0.010056775320344857</v>
       </c>
       <c r="I4" s="0">
-        <v>0.018078030462397421</v>
+        <v>0.098712917842206357</v>
       </c>
       <c r="J4" s="0">
-        <v>1.1596948448392532e-05</v>
+        <v>0.067866084315256883</v>
       </c>
       <c r="K4" s="0">
-        <v>-2.811917477957282e-05</v>
+        <v>-0.0043579644951129981</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B5" s="0">
-        <v>0.37612488087858736</v>
+        <v>0.27969653077730205</v>
       </c>
       <c r="C5" s="0">
         <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>-0.016126474941842894</v>
+        <v>0.021974718140459808</v>
       </c>
       <c r="E5" s="0">
-        <v>0.0028315545873402888</v>
+        <v>-0.017335230934012388</v>
       </c>
       <c r="F5" s="0">
-        <v>-0.0010515570433003176</v>
+        <v>-0.30358526355712673</v>
       </c>
       <c r="G5" s="0">
-        <v>0.011303132070250917</v>
+        <v>0.011576210255504423</v>
       </c>
       <c r="H5" s="0">
-        <v>-0.00091531031657483049</v>
+        <v>-0.0027566847478400379</v>
       </c>
       <c r="I5" s="0">
-        <v>0.05645761227097934</v>
+        <v>-0.0142890870565447</v>
       </c>
       <c r="J5" s="0">
         <v>0</v>
       </c>
       <c r="K5" s="0">
-        <v>0.0012190543318466029</v>
+        <v>-0.001975714277650642</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B6" s="0">
-        <v>0.34646286501084489</v>
+        <v>0.223861104771157</v>
       </c>
       <c r="C6" s="0">
-        <v>-0.076554256887560762</v>
+        <v>0.010287819838922782</v>
       </c>
       <c r="D6" s="0">
         <v>0</v>
       </c>
       <c r="E6" s="0">
-        <v>-0.00019065460388359564</v>
+        <v>0.0079998235900632635</v>
       </c>
       <c r="F6" s="0">
-        <v>0.00080992227450875592</v>
+        <v>-0.0073367079466580727</v>
       </c>
       <c r="G6" s="0">
         <v>0</v>
       </c>
       <c r="H6" s="0">
-        <v>0.0010225564104789995</v>
+        <v>-0.022120259021892876</v>
       </c>
       <c r="I6" s="0">
-        <v>0.045192405609450481</v>
+        <v>-0.045433160924870888</v>
       </c>
       <c r="J6" s="0">
         <v>0</v>
       </c>
       <c r="K6" s="0">
-        <v>5.8011329263640832e-05</v>
+        <v>0.00076705845829072583</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B7" s="0">
-        <v>0.28240490844011656</v>
+        <v>0.02261423482896624</v>
       </c>
       <c r="C7" s="0">
         <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>-0.11053202449328432</v>
+        <v>0.096833168159151189</v>
       </c>
       <c r="E7" s="0">
-        <v>0.049314822541931626</v>
+        <v>0.041896681731447623</v>
       </c>
       <c r="F7" s="0">
-        <v>-0.0070387180983145113</v>
+        <v>-0.32462595824466861</v>
       </c>
       <c r="G7" s="0">
-        <v>0.0080649559752040013</v>
+        <v>-0.016711463629417434</v>
       </c>
       <c r="H7" s="0">
-        <v>-0.00070612734737192579</v>
+        <v>0</v>
       </c>
       <c r="I7" s="0">
-        <v>0.0013272509294573378</v>
+        <v>0</v>
       </c>
       <c r="J7" s="0">
         <v>0</v>
       </c>
       <c r="K7" s="0">
-        <v>-0.0044881160783505347</v>
+        <v>0.0013607020412964577</v>
       </c>
     </row>
     <row r="8">

</xml_diff>